<commit_message>
all right remaark off time
</commit_message>
<xml_diff>
--- a/Paint Booth Data Logging V1.xlsx
+++ b/Paint Booth Data Logging V1.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Mapping" sheetId="2" r:id="rId2"/>
     <sheet name="Format" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="154">
   <si>
     <t>12-06-23 06:27:52(AM)</t>
   </si>
@@ -572,7 +572,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -588,6 +588,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -656,7 +668,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -770,9 +782,6 @@
     <xf numFmtId="21" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -780,14 +789,14 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -807,6 +816,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1146,7 +1164,6 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
       </c:pie3DChart>
       <c:spPr>
         <a:noFill/>
@@ -1223,7 +1240,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1249,7 +1266,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9A42E05C-5E67-49D7-8522-F8A365C5CC04}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A42E05C-5E67-49D7-8522-F8A365C5CC04}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1525,7 +1542,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1554,11 +1571,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="24"/>
@@ -1659,7 +1676,7 @@
         <f>B8/B9*1000000</f>
         <v>5067.5675675675675</v>
       </c>
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="48" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1671,7 +1688,7 @@
         <f>B10/B11*100</f>
         <v>6.5217391304347823</v>
       </c>
-      <c r="C13" s="49"/>
+      <c r="C13" s="48"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="29" t="s">
@@ -1681,7 +1698,7 @@
         <f>B9/B7*100</f>
         <v>98.666666666666671</v>
       </c>
-      <c r="C14" s="49"/>
+      <c r="C14" s="48"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="29" t="s">
@@ -1691,7 +1708,7 @@
         <f>(B11-B10)/B11*100</f>
         <v>93.478260869565219</v>
       </c>
-      <c r="C15" s="49"/>
+      <c r="C15" s="48"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="29" t="s">
@@ -1701,7 +1718,7 @@
         <f>(B9-B8)/B9*100</f>
         <v>99.493243243243242</v>
       </c>
-      <c r="C16" s="49"/>
+      <c r="C16" s="48"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="29" t="s">
@@ -1711,7 +1728,7 @@
         <f>B14*B15*B16/10000</f>
         <v>91.764492753623188</v>
       </c>
-      <c r="C17" s="49"/>
+      <c r="C17" s="48"/>
     </row>
     <row r="18" spans="1:4" ht="14.4">
       <c r="A18" s="18"/>
@@ -1719,12 +1736,12 @@
       <c r="C18" s="20"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="50"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="27.6">
       <c r="A20" s="1" t="s">
@@ -1898,10 +1915,10 @@
       <c r="D32" s="8"/>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="50" t="s">
+      <c r="A33" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="50"/>
+      <c r="B33" s="49"/>
       <c r="C33" s="7" t="s">
         <v>26</v>
       </c>
@@ -2024,8 +2041,8 @@
       <c r="C41" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F41" s="47"/>
-      <c r="G41" s="47"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="46"/>
       <c r="H41" s="15"/>
       <c r="I41" s="16"/>
     </row>
@@ -2127,24 +2144,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="37"/>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
       <c r="F3" s="37"/>
       <c r="G3" s="37"/>
     </row>
@@ -2183,14 +2200,14 @@
       <c r="A7" s="32">
         <v>2</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="43" t="s">
         <v>72</v>
       </c>
       <c r="D7" s="32"/>
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="42" t="s">
         <v>68</v>
       </c>
       <c r="F7" s="31" t="s">
@@ -2204,10 +2221,10 @@
       <c r="A8" s="32">
         <v>3</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="44" t="s">
         <v>148</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="43" t="s">
         <v>73</v>
       </c>
       <c r="D8" s="32"/>
@@ -2223,16 +2240,16 @@
         <v>131</v>
       </c>
       <c r="D9" s="32"/>
-      <c r="F9" s="51" t="s">
+      <c r="F9" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="G9" s="51"/>
+      <c r="G9" s="50"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="42">
+      <c r="A10" s="41">
         <v>5</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="44" t="s">
         <v>150</v>
       </c>
       <c r="C10" s="32" t="s">
@@ -2246,7 +2263,7 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="45">
+      <c r="A11" s="43">
         <v>6</v>
       </c>
       <c r="B11" s="34" t="s">
@@ -2263,7 +2280,7 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="42">
+      <c r="A12" s="41">
         <v>7</v>
       </c>
       <c r="B12" s="34" t="s">
@@ -2280,7 +2297,7 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="45">
+      <c r="A13" s="43">
         <v>8</v>
       </c>
       <c r="B13" s="34" t="s">
@@ -2294,7 +2311,7 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="42">
+      <c r="A14" s="41">
         <v>9</v>
       </c>
       <c r="B14" s="34" t="s">
@@ -2308,7 +2325,7 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="45">
+      <c r="A15" s="43">
         <v>10</v>
       </c>
       <c r="B15" s="34" t="s">
@@ -2322,7 +2339,7 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="42">
+      <c r="A16" s="41">
         <v>11</v>
       </c>
       <c r="B16" s="34" t="s">
@@ -2336,7 +2353,7 @@
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="45">
+      <c r="A17" s="43">
         <v>12</v>
       </c>
       <c r="B17" s="34" t="s">
@@ -2372,10 +2389,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:AC10"/>
+  <dimension ref="A2:AC19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -2407,38 +2424,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:29">
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
     </row>
     <row r="3" spans="1:29" ht="28.8">
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="41" t="s">
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="F3" s="31" t="s">
+      <c r="F3" s="53" t="s">
         <v>89</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="H3" s="31" t="s">
+      <c r="H3" s="53" t="s">
         <v>89</v>
       </c>
-      <c r="I3" s="31" t="s">
+      <c r="I3" s="53" t="s">
         <v>130</v>
       </c>
-      <c r="J3" s="31" t="s">
+      <c r="J3" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="K3" s="31" t="s">
+      <c r="K3" s="53" t="s">
         <v>90</v>
       </c>
       <c r="L3" s="31" t="s">
@@ -2447,22 +2464,22 @@
       <c r="M3" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="N3" s="31" t="s">
+      <c r="N3" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="O3" s="31" t="s">
+      <c r="O3" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="P3" s="31" t="s">
+      <c r="P3" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="Q3" s="31" t="s">
+      <c r="Q3" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="R3" s="31" t="s">
+      <c r="R3" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="S3" s="31" t="s">
+      <c r="S3" s="53" t="s">
         <v>90</v>
       </c>
       <c r="T3" s="31" t="s">
@@ -2551,7 +2568,7 @@
       <c r="S4" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="T4" s="31" t="s">
+      <c r="T4" s="45" t="s">
         <v>99</v>
       </c>
       <c r="U4" s="31" t="s">
@@ -2865,6 +2882,348 @@
       <c r="AB10" s="31"/>
       <c r="AC10" s="31"/>
     </row>
+    <row r="14" spans="1:29" ht="28.8">
+      <c r="B14" s="53"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="E14" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="F14" s="53" t="s">
+        <v>89</v>
+      </c>
+      <c r="G14" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="H14" s="53" t="s">
+        <v>89</v>
+      </c>
+      <c r="I14" s="53" t="s">
+        <v>130</v>
+      </c>
+      <c r="J14" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="K14" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="L14" s="53" t="s">
+        <v>96</v>
+      </c>
+      <c r="M14" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="N14" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="O14" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="P14" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q14" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="R14" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="S14" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="T14" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="U14" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="V14" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="W14" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="X14" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y14" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z14" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA14" s="55" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" ht="43.2">
+      <c r="B15" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="E15" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="F15" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="H15" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="I15" s="45" t="s">
+        <v>118</v>
+      </c>
+      <c r="J15" s="45" t="s">
+        <v>152</v>
+      </c>
+      <c r="K15" s="45" t="s">
+        <v>153</v>
+      </c>
+      <c r="L15" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="M15" s="45" t="s">
+        <v>125</v>
+      </c>
+      <c r="N15" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="O15" s="45" t="s">
+        <v>127</v>
+      </c>
+      <c r="P15" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q15" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="R15" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="S15" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="T15" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="U15" s="45" t="s">
+        <v>110</v>
+      </c>
+      <c r="V15" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="W15" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="X15" s="45" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y15" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="Z15" s="45" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA15" s="45" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29">
+      <c r="B16" s="45"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="E16" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="F16" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="G16" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="H16" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="I16" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="J16" s="45"/>
+      <c r="K16" s="45"/>
+      <c r="L16" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="M16" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="N16" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="O16" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="P16" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q16" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="R16" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="S16" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="T16" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="U16" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="V16" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="W16" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="X16" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y16" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z16" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA16" s="45" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="2:27">
+      <c r="B17" s="39">
+        <v>45751</v>
+      </c>
+      <c r="C17" s="40">
+        <v>0.43767361111111114</v>
+      </c>
+      <c r="D17" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" s="45">
+        <v>1.7</v>
+      </c>
+      <c r="F17" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="G17" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="H17" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="I17" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="J17" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="K17" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="L17" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="M17" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="N17" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="O17" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="P17" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q17" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="R17" s="45" t="s">
+        <v>113</v>
+      </c>
+      <c r="S17" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="T17" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="U17" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="V17" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="W17" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="X17" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="Y17" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z17" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA17" s="45" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="2:27">
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="45"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="45"/>
+      <c r="M18" s="45"/>
+      <c r="N18" s="45"/>
+      <c r="O18" s="45"/>
+      <c r="P18" s="45"/>
+      <c r="Q18" s="45"/>
+      <c r="R18" s="45"/>
+      <c r="S18" s="45"/>
+      <c r="T18" s="45"/>
+      <c r="U18" s="45"/>
+      <c r="V18" s="45"/>
+      <c r="W18" s="45"/>
+      <c r="X18" s="45"/>
+      <c r="Y18" s="45"/>
+      <c r="Z18" s="45"/>
+      <c r="AA18" s="45"/>
+    </row>
+    <row r="19" spans="2:27">
+      <c r="T19" s="38" t="e">
+        <f>R18-R17</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>